<commit_message>
ontoneo part of error from ro import
</commit_message>
<xml_diff>
--- a/ontologies/loinc_etc/loinc_obo_assay_template_more_harmonious.xlsx
+++ b/ontologies/loinc_etc/loinc_obo_assay_template_more_harmonious.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Miller\Turbo-Ontology\ontologies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Miller\Turbo-Ontology\ontologies\loinc_etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,6 +24,31 @@
     <author>Mark Miller</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mark Miller:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Chris left the IRIs out of his versions
+ADD GFRs back in</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
@@ -166,7 +191,9 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-move true analytes here if OBI consensus is against adding a measurand column or changing the analyte column to a measurand column</t>
+move true analytes here if OBI consensus is against adding a measurand column or changing the analyte column to a measurand column
+check validation errors and move measurands
+CS: My understanding of the OBI consensus is that we have two columns: one for analyte and one for measurand when it is not an analyte. </t>
         </r>
       </text>
     </comment>
@@ -290,7 +317,9 @@
           <t xml:space="preserve">
 Mark wants a general purpose column for annotating each term row with an external URI. rdfs:seeAlso is not currently a column in assays.tsv and may not be the best choice anyway.
 Also have to look into licensure. 
-Mark would like to keep all of this in one artifact if possible</t>
+Mark would like to keep all of this in one artifact if possible
+CS: see also is being used by others to refer to things like papers or websites. We should use a database_cross_reference as is done by other OBOF ontologies linking to clinical terminologies
+</t>
         </r>
       </text>
     </comment>
@@ -460,9 +489,6 @@
     <t>C (has_specified_input some %) and (realizes some ('measurand role' and ('inheres in' some %)))</t>
   </si>
   <si>
-    <t>AI see also</t>
-  </si>
-  <si>
     <t>http://transformunify.org/ontologies/TURBO_0010721</t>
   </si>
   <si>
@@ -626,6 +652,9 @@
   </si>
   <si>
     <t>arbitrary units per 24 hours datum</t>
+  </si>
+  <si>
+    <t>AI http://www.geneontology.org/formats/oboInOwl#hasDbXref</t>
   </si>
 </sst>
 </file>
@@ -1465,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AB31" sqref="AB31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,280 +1696,280 @@
         <v>52</v>
       </c>
       <c r="AB2" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>55</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>56</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>57</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q4" t="s">
         <v>60</v>
       </c>
-      <c r="B4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" t="s">
-        <v>87</v>
-      </c>
-      <c r="L4" t="s">
-        <v>55</v>
-      </c>
-      <c r="N4" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB4" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>60</v>
+      </c>
+      <c r="R5" t="s">
         <v>63</v>
       </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
-      <c r="L5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>61</v>
-      </c>
       <c r="W5" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA5" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB5" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L6" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" t="s">
         <v>66</v>
       </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-      <c r="N6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>67</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA6" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB6" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>89</v>
+      </c>
+      <c r="L7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" t="s">
         <v>70</v>
       </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" t="s">
-        <v>90</v>
-      </c>
-      <c r="L7" t="s">
-        <v>55</v>
-      </c>
-      <c r="N7" t="s">
-        <v>56</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" t="s">
+        <v>67</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB7" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>67</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB7" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>66</v>
+      </c>
+      <c r="R8" t="s">
         <v>73</v>
       </c>
-      <c r="B8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>91</v>
-      </c>
-      <c r="L8" t="s">
-        <v>55</v>
-      </c>
-      <c r="N8" t="s">
-        <v>56</v>
-      </c>
-      <c r="P8" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>67</v>
-      </c>
       <c r="W8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB8" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="AB8" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="L9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>56</v>
+      </c>
+      <c r="R9" t="s">
         <v>76</v>
       </c>
-      <c r="B9" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" t="s">
-        <v>92</v>
-      </c>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N9" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>57</v>
-      </c>
       <c r="W9" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB9" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="AB9" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" t="s">
+        <v>55</v>
+      </c>
+      <c r="P10" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" t="s">
+        <v>80</v>
+      </c>
+      <c r="W10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B10" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" t="s">
-        <v>93</v>
-      </c>
-      <c r="L10" t="s">
-        <v>55</v>
-      </c>
-      <c r="N10" t="s">
-        <v>56</v>
-      </c>
-      <c r="P10" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>61</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA10" t="s">
+      <c r="AB10" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P11" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" t="s">
         <v>83</v>
       </c>
-      <c r="B11" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
-      <c r="L11" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" t="s">
-        <v>56</v>
-      </c>
-      <c r="P11" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>61</v>
-      </c>
       <c r="W11" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA11" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB11" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>